<commit_message>
Tao folder lam viec cho DEV
</commit_message>
<xml_diff>
--- a/FW_CM_Plan.xlsx
+++ b/FW_CM_Plan.xlsx
@@ -1463,8 +1463,8 @@
   <sheetPr/>
   <dimension ref="A1:K976"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.45" defaultRowHeight="15" customHeight="1"/>

</xml_diff>